<commit_message>
some additional formating changes
</commit_message>
<xml_diff>
--- a/Images/data_additional.xlsx
+++ b/Images/data_additional.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zcftaeu_ucl_ac_uk/Documents/Documents/University/YearM_T2/CASA0023/GroupPresentation/desert-roses/Images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{E081BB90-178A-4ADB-A15E-0832B53FC19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{505AE583-69E3-4212-B17F-3EB4AB14CEB2}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="8_{E081BB90-178A-4ADB-A15E-0832B53FC19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EEFB59F-ED50-4BF6-9E6A-D7A1BB8C6320}"/>
   <bookViews>
-    <workbookView xWindow="63000" yWindow="2655" windowWidth="23805" windowHeight="9960" xr2:uid="{9FC9B43F-F867-4683-A08A-E0DDCD3D78E4}"/>
+    <workbookView xWindow="62595" yWindow="2655" windowWidth="23805" windowHeight="9960" xr2:uid="{9FC9B43F-F867-4683-A08A-E0DDCD3D78E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -495,7 +495,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>